<commit_message>
Attempt to fix downloadexcel Reloading
</commit_message>
<xml_diff>
--- a/server/files/orderExport.xlsx
+++ b/server/files/orderExport.xlsx
@@ -378,7 +378,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Receivers"/>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -397,18 +397,21 @@
         <v>VAT NUMBER</v>
       </c>
       <c r="E1" t="str">
+        <v>DOY NUMBER</v>
+      </c>
+      <c r="F1" t="str">
         <v>ADDRESS</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>ZIP CODE</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>LOCATION</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>PHONE #1</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>PHONE #2</v>
       </c>
     </row>
@@ -419,14 +422,20 @@
       <c r="B2" t="str">
         <v>ΒΑΣΙΛΕΙΟΥ  ΦΩΤΙΟΣ</v>
       </c>
-      <c r="E2" t="str">
+      <c r="D2" t="str">
+        <v>052368639</v>
+      </c>
+      <c r="F2" t="str">
         <v>ΧΡΙΣΤΟΒΑΣΙΛΗ 1</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>46100</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>ΗΓΟΥΜΕΝΙΤΣΑ</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2665027775</v>
       </c>
     </row>
     <row r="3">
@@ -436,14 +445,20 @@
       <c r="B3" t="str">
         <v>ΝΟΣΟΚΟΜΕΙΟ ΣΑΜΟΥ</v>
       </c>
-      <c r="E3" t="str">
+      <c r="D3" t="str">
+        <v>999340688</v>
+      </c>
+      <c r="F3" t="str">
         <v>ΣΥΝ/ΡΧΟΥ ΚΕΦΑΛΟΠΟΥΛΟΥ 17</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>83100</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>ΣΑΜΟΣ</v>
+      </c>
+      <c r="I3" t="str">
+        <v>2273083150</v>
       </c>
     </row>
     <row r="4">
@@ -453,13 +468,16 @@
       <c r="B4" t="str">
         <v>SPOT4TONER Ι Κ Ε</v>
       </c>
-      <c r="E4" t="str">
+      <c r="D4" t="str">
+        <v>800839540</v>
+      </c>
+      <c r="F4" t="str">
         <v>ΑΓΓΕΛΑΚΗ 3</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <v>54621</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>ΘΕΣΣΑΛΟΝΙΚΗ</v>
       </c>
     </row>
@@ -470,14 +488,20 @@
       <c r="B5" t="str">
         <v>ΤΑΤΣΗΣ  ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E5" t="str">
+      <c r="D5" t="str">
+        <v>134312928</v>
+      </c>
+      <c r="F5" t="str">
         <v>ΦΛΕΜΙΝΓΚ ΚΑΙ ΠΕΡΙΦ ΟΔΟΣ 0</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <v>47100</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>ΑΡΤΑ</v>
+      </c>
+      <c r="I5" t="str">
+        <v>2681071591</v>
       </c>
     </row>
     <row r="6">
@@ -487,13 +511,16 @@
       <c r="B6" t="str">
         <v>ΕΠΙΜΕΛΗΤΗΡΙΟ ΙΩΑΝΝΙΝΩΝ</v>
       </c>
-      <c r="E6" t="str">
+      <c r="D6" t="str">
+        <v>090141710</v>
+      </c>
+      <c r="F6" t="str">
         <v>ΠΟΥΤΕΤΣΗ 14</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <v>45333</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>ΙΩΑΝΝΙΝΑ</v>
       </c>
     </row>
@@ -504,10 +531,13 @@
       <c r="B7" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΚΕΡΚΥΡΑΣ</v>
       </c>
-      <c r="E7" t="str">
+      <c r="D7" t="str">
+        <v>999360466</v>
+      </c>
+      <c r="F7" t="str">
         <v>ΚΟΝΤΟΚΑΛΙ</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <v>49100</v>
       </c>
     </row>
@@ -518,11 +548,20 @@
       <c r="B8" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΑΝΑΤΟΛΙΚΗΣ ΑΧΑΪΑΣ</v>
       </c>
-      <c r="E8" t="str">
+      <c r="D8" t="str">
+        <v>999894869</v>
+      </c>
+      <c r="F8" t="str">
         <v>ΑΝΩ ΒΟΥΛΩΜΕΝΟ</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <v>25100</v>
+      </c>
+      <c r="I8" t="str">
+        <v>2691059489</v>
+      </c>
+      <c r="J8" t="str">
+        <v>2691059491</v>
       </c>
     </row>
     <row r="9">
@@ -532,11 +571,20 @@
       <c r="B9" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΒΟΛΟΥ</v>
       </c>
-      <c r="E9" t="str">
+      <c r="D9" t="str">
+        <v>999501452</v>
+      </c>
+      <c r="F9" t="str">
         <v>ΠΟΛΥΜΕΡΗ 134</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <v>38222</v>
+      </c>
+      <c r="I9" t="str">
+        <v>2421351117</v>
+      </c>
+      <c r="J9" t="str">
+        <v>2421351156</v>
       </c>
     </row>
     <row r="10">
@@ -546,14 +594,23 @@
       <c r="B10" t="str">
         <v>ΛΑΒΡΑΝΟΣ  ΧΡΙΣΤΟΔΟΥΛΟΣ ΣΠΥΡΙΔΩΝ</v>
       </c>
-      <c r="E10" t="str">
+      <c r="D10" t="str">
+        <v>135673258</v>
+      </c>
+      <c r="F10" t="str">
         <v>ΑΝΩ ΜΕΣΟΓΓΗ 00</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <v>49080</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <v>ΛΕΥΚΙΜΜΗ</v>
+      </c>
+      <c r="I10" t="str">
+        <v>26610 75233</v>
+      </c>
+      <c r="J10" t="str">
+        <v>694 47 47 290</v>
       </c>
     </row>
     <row r="11">
@@ -563,13 +620,16 @@
       <c r="B11" t="str">
         <v>ΥΠΟΥΡΓΕΙΟ ΔΙΚΑΙΟΣΥΝΗΣ</v>
       </c>
-      <c r="E11" t="str">
+      <c r="D11" t="str">
+        <v>090169674</v>
+      </c>
+      <c r="F11" t="str">
         <v>ΜΕΣΟΓΕΙΩΝ 96</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <v>11527</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <v>ΑΘΗΝΑ</v>
       </c>
     </row>
@@ -580,14 +640,20 @@
       <c r="B12" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΚΑΡΔΙΤΣΑΣ</v>
       </c>
-      <c r="E12" t="str">
+      <c r="D12" t="str">
+        <v>999091563</v>
+      </c>
+      <c r="F12" t="str">
         <v>ΤΕΡΜΑ ΤΑΥΡΩΠΟΥ 0</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <v>43100</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <v>ΚΑΡΔΙΤΣΑ</v>
+      </c>
+      <c r="I12" t="str">
+        <v>2441351195</v>
       </c>
     </row>
     <row r="13">
@@ -597,13 +663,16 @@
       <c r="B13" t="str">
         <v>ΔΙΟΙΚ 6ΗΣ ΥΓΕΙΟΝ ΠΕΡΙΦ ΠΕΛΛΟΠ. ΙΩΝΙΩΝ ΔΥ</v>
       </c>
-      <c r="E13" t="str">
+      <c r="D13" t="str">
+        <v>999100797</v>
+      </c>
+      <c r="F13" t="str">
         <v>ΥΠΑΤΗΣ 1</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <v>26441</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <v>ΠΑΤΡΑ</v>
       </c>
     </row>
@@ -614,14 +683,20 @@
       <c r="B14" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΚΕΝΤΡΟ ΥΓΕΙΑΣ ΛΗΜΝΟΥ</v>
       </c>
-      <c r="E14" t="str">
+      <c r="D14" t="str">
+        <v>997255081</v>
+      </c>
+      <c r="F14" t="str">
         <v>ΜΥΡΙΝΑ 0</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <v>81400</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <v>ΜΥΡΙΝΑ</v>
+      </c>
+      <c r="I14" t="str">
+        <v>2254350129</v>
       </c>
     </row>
     <row r="15">
@@ -631,14 +706,23 @@
       <c r="B15" t="str">
         <v>ΒΡΥΣΗΣ ΙΩΑΝΝΗΣ ΚΑΙ ΣΙΑ ΟΕ</v>
       </c>
-      <c r="E15" t="str">
+      <c r="D15" t="str">
+        <v>999858963</v>
+      </c>
+      <c r="F15" t="str">
         <v>ΚΥΠΡΟΥ 47</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <v>46100</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <v>ΗΓΟΥΜΕΝΙΤΣΑ</v>
+      </c>
+      <c r="I15" t="str">
+        <v>2665021345</v>
+      </c>
+      <c r="J15" t="str">
+        <v>6942471543</v>
       </c>
     </row>
     <row r="16">
@@ -648,14 +732,20 @@
       <c r="B16" t="str">
         <v>Γ ΖΑΒΑΝΤΙΑΣ-Χ ΚΑΡΑΦΥΛΛΙΔΗΣ ΟΕ</v>
       </c>
-      <c r="E16" t="str">
+      <c r="D16" t="str">
+        <v>084171745</v>
+      </c>
+      <c r="F16" t="str">
         <v>ΘΕΣΣΑΛΟΝΙΚΗΣ 31</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <v>60100</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <v>ΚΑΤΕΡΙΝΗ</v>
+      </c>
+      <c r="I16" t="str">
+        <v>2351078110</v>
       </c>
     </row>
     <row r="17">
@@ -665,14 +755,20 @@
       <c r="B17" t="str">
         <v>ΠΑΡΔΑΣ ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E17" t="str">
+      <c r="D17" t="str">
+        <v>134811987</v>
+      </c>
+      <c r="F17" t="str">
         <v>20 ΟΚΤΩΒΡΙΟΥ 4</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <v>58100</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <v>ΓΙΑΝΝΙΤΣΑ</v>
+      </c>
+      <c r="I17" t="str">
+        <v>2382028158</v>
       </c>
     </row>
     <row r="18">
@@ -682,14 +778,23 @@
       <c r="B18" t="str">
         <v>PRIME POWER ΜΟΝΟΠΡΟΣΩΠΗ ΙΚΕ</v>
       </c>
-      <c r="E18" t="str">
+      <c r="D18" t="str">
+        <v>800481628</v>
+      </c>
+      <c r="F18" t="str">
         <v>ΙΛΙΟΥ ΚΑΙ Μ ΜΑΥΡΟΓΕΝΟΥΣ 1</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <v>16674</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <v>ΓΛΥΦΑΔΑ</v>
+      </c>
+      <c r="I18" t="str">
+        <v>2155105070</v>
+      </c>
+      <c r="J18" t="str">
+        <v>2109480958</v>
       </c>
     </row>
     <row r="19">
@@ -699,14 +804,20 @@
       <c r="B19" t="str">
         <v>ΜΩΡΑΙΤΗ  ΜΑΡΙΑ ΑΘΑΝΑΣΙΟΣ</v>
       </c>
-      <c r="E19" t="str">
+      <c r="D19" t="str">
+        <v>055472412</v>
+      </c>
+      <c r="F19" t="str">
         <v>ΑΓΙΑΣ ΣΟΦΙΑΣ 15</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <v>26441</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <v>ΠΑΤΡΑ</v>
+      </c>
+      <c r="I19" t="str">
+        <v>2610433413</v>
       </c>
     </row>
     <row r="20">
@@ -716,14 +827,20 @@
       <c r="B20" t="str">
         <v>ΓΑΒΡΙΗΛΙΔΗΣ  ΑΝΕΣΤΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</v>
       </c>
-      <c r="E20" t="str">
+      <c r="D20" t="str">
+        <v>066515981</v>
+      </c>
+      <c r="F20" t="str">
         <v>ΑΜΕΡ ΕΡΥΘΡΟΥ ΣΤΑΥΡΟΥ 104</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <v>65201</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <v>ΚΑΒΑΛΑ</v>
+      </c>
+      <c r="I20" t="str">
+        <v>2510222222</v>
       </c>
     </row>
     <row r="21">
@@ -733,14 +850,23 @@
       <c r="B21" t="str">
         <v>ΚΑΝΤΑΡΕΛΗΣ ΗΛΙΑΣ</v>
       </c>
-      <c r="E21" t="str">
+      <c r="D21" t="str">
+        <v>119085590</v>
+      </c>
+      <c r="F21" t="str">
         <v>ΑΧΑΡΑΒΗ</v>
       </c>
-      <c r="F21" t="str">
+      <c r="G21" t="str">
         <v>49081</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <v>ΚΑΡΟΥΣΑΔΕΣ</v>
+      </c>
+      <c r="I21" t="str">
+        <v>2663064381</v>
+      </c>
+      <c r="J21" t="str">
+        <v>6945993231</v>
       </c>
     </row>
     <row r="22">
@@ -750,14 +876,23 @@
       <c r="B22" t="str">
         <v>ΖΑΡΙΦΗΣ  ΜΙΧΑΗΛ ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E22" t="str">
+      <c r="D22" t="str">
+        <v>077288320</v>
+      </c>
+      <c r="F22" t="str">
         <v>ΛΕΩΦΟΡΟΣ ΔΗΜΟΚΡΑΤΙΑΣ 57-59</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <v>18755</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <v>ΚΕΡΑΤΣΙΝΙ</v>
+      </c>
+      <c r="I22" t="str">
+        <v>2104629664</v>
+      </c>
+      <c r="J22" t="str">
+        <v>694 838 1318</v>
       </c>
     </row>
     <row r="23">
@@ -767,14 +902,20 @@
       <c r="B23" t="str">
         <v>Γ.Ν ΙΠΠΟΚΡΑΤΕΙΟ ΘΕΣ/ΝΙΚΗΣ</v>
       </c>
-      <c r="E23" t="str">
+      <c r="D23" t="str">
+        <v>999432325</v>
+      </c>
+      <c r="F23" t="str">
         <v>ΚΩΝΣΤΑΝΤΙΝΟΥΠΟΛΕΩΣ 49</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <v>54641</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <v>ΘΕΣΣΑΛΟΝΙΚΗ</v>
+      </c>
+      <c r="I23" t="str">
+        <v>231331261</v>
       </c>
     </row>
     <row r="24">
@@ -784,14 +925,20 @@
       <c r="B24" t="str">
         <v>ΚΑΚΟΛΥΡΗΣ ΓΡΗΓΟΡΗΣ</v>
       </c>
-      <c r="E24" t="str">
+      <c r="D24" t="str">
+        <v>046314215</v>
+      </c>
+      <c r="F24" t="str">
         <v>ΦΙΛΙΚΗΣ ΕΤΑΙΡΕΙΑΣ 2</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <v>27200</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <v>ΑΜΑΛΙΑΔΑ</v>
+      </c>
+      <c r="I24" t="str">
+        <v>2622021770</v>
       </c>
     </row>
     <row r="25">
@@ -801,14 +948,20 @@
       <c r="B25" t="str">
         <v>ΧΡΥΣΑΓΗΣ  ΝΙΚΟΛΑΟΣ</v>
       </c>
-      <c r="E25" t="str">
+      <c r="D25" t="str">
+        <v>102676914</v>
+      </c>
+      <c r="F25" t="str">
         <v>ΠΕΡΣΕΦΩΝΗΣ 10</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <v>66100</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <v>ΔΡΑΜΑ</v>
+      </c>
+      <c r="I25" t="str">
+        <v>6937352410</v>
       </c>
     </row>
     <row r="26">
@@ -818,14 +971,23 @@
       <c r="B26" t="str">
         <v>ΕΥΑΓΓΕΛΟΣ ΔΑΝΙΗΛ ΚΑΙ ΣΙΑ ΟΕ</v>
       </c>
-      <c r="E26" t="str">
+      <c r="D26" t="str">
+        <v>800187440</v>
+      </c>
+      <c r="F26" t="str">
         <v>ΛΕΩΦΟΡΟΣ ΔΗΜΟΚΡΑΤΙΑΣ 20</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <v>81400</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <v>ΜΥΡΙΝΑ - ΛΗΜΝΟΣ</v>
+      </c>
+      <c r="I26" t="str">
+        <v>2254024314</v>
+      </c>
+      <c r="J26" t="str">
+        <v>6942404436</v>
       </c>
     </row>
     <row r="27">
@@ -835,14 +997,20 @@
       <c r="B27" t="str">
         <v>ΓΕΩΡΓΙΟΣ ΜΠΑΛΗΣ-ΖΗΝΟΒΙΑ ΜΠΑΛΗ ΟΕ</v>
       </c>
-      <c r="E27" t="str">
+      <c r="D27" t="str">
+        <v>082648231</v>
+      </c>
+      <c r="F27" t="str">
         <v>ΔΑΜΑΡΕΩΣ 177</v>
       </c>
-      <c r="F27" t="str">
+      <c r="G27" t="str">
         <v>11632</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <v>ΑΘΗΝΑ</v>
+      </c>
+      <c r="I27" t="str">
+        <v>2107019503</v>
       </c>
     </row>
     <row r="28">
@@ -852,14 +1020,23 @@
       <c r="B28" t="str">
         <v>ΚΙΝΤΩΝΗ  ΠΑΝΑΓΙΩΤΑ</v>
       </c>
-      <c r="E28" t="str">
+      <c r="D28" t="str">
+        <v>068001639</v>
+      </c>
+      <c r="F28" t="str">
         <v>ΚΑΝΕΛΛΟΠΟΥΛΟΥ ΚΑΙ ΣΟΛΙΩΤΗ ΝΙΚΟΛΑΟΥ ΓΩΝΙΑ</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <v>25100</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <v>ΑΙΓΙΟ</v>
+      </c>
+      <c r="I28" t="str">
+        <v>2691024324</v>
+      </c>
+      <c r="J28" t="str">
+        <v>6986215161</v>
       </c>
     </row>
     <row r="29">
@@ -869,14 +1046,23 @@
       <c r="B29" t="str">
         <v>ΕΛΕΥΘΕΡΙΑΔΗΣ  ΧΑΡΑΛΑΜΠΟΣ</v>
       </c>
-      <c r="E29" t="str">
+      <c r="D29" t="str">
+        <v>142076872</v>
+      </c>
+      <c r="F29" t="str">
         <v>Λ. ΔΗΜΟΚΡΑΤΙΑΣ &amp; ΗΡΩΩΝ ΠΟΛΥΤΕΧΝΕΙΟΥ 27</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <v>19300</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <v>ΑΣΠΡΟΠΥΡΓΟΣ</v>
+      </c>
+      <c r="I29" t="str">
+        <v>6970896967</v>
+      </c>
+      <c r="J29" t="str">
+        <v>2155150270</v>
       </c>
     </row>
     <row r="30">
@@ -886,14 +1072,20 @@
       <c r="B30" t="str">
         <v>ΜΑΝΙΟΣ  ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E30" t="str">
+      <c r="D30" t="str">
+        <v>036740915</v>
+      </c>
+      <c r="F30" t="str">
         <v>ΝΙΚΟΥ ΚΑΖΑΝΤΖΑΚΗ 2</v>
       </c>
-      <c r="F30" t="str">
+      <c r="G30" t="str">
         <v>85100</v>
       </c>
-      <c r="G30" t="str">
+      <c r="H30" t="str">
         <v>ΡΟΔΟΣ</v>
+      </c>
+      <c r="I30" t="str">
+        <v>2241036626</v>
       </c>
     </row>
     <row r="31">
@@ -903,14 +1095,23 @@
       <c r="B31" t="str">
         <v>ΤΣΕΡΕΜΕΓΚΛΗΣ  ΠΑΝΑΓΙΩΤΗΣ ΑΝΔΡΕΑΣ</v>
       </c>
-      <c r="E31" t="str">
+      <c r="D31" t="str">
+        <v>126524730</v>
+      </c>
+      <c r="F31" t="str">
         <v>ΥΨΗΛΑΝΤΟΥ 133</v>
       </c>
-      <c r="F31" t="str">
+      <c r="G31" t="str">
         <v>26221</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <v>ΠΑΤΡΑ</v>
+      </c>
+      <c r="I31" t="str">
+        <v>2610223378</v>
+      </c>
+      <c r="J31" t="str">
+        <v>6972052191</v>
       </c>
     </row>
     <row r="32">
@@ -920,14 +1121,23 @@
       <c r="B32" t="str">
         <v>ΠΑΠΑΙΩΑΝΝΟΥ  ΑΠΟΣΤΟΛΟΣ</v>
       </c>
-      <c r="E32" t="str">
+      <c r="D32" t="str">
+        <v>036067124</v>
+      </c>
+      <c r="F32" t="str">
         <v>Ν ΜΠΟΤΣΑΡΗ 34</v>
       </c>
-      <c r="F32" t="str">
+      <c r="G32" t="str">
         <v>30300</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <v>ΝΑΥΠΑΚΤΟΣ</v>
+      </c>
+      <c r="I32" t="str">
+        <v>2634026005</v>
+      </c>
+      <c r="J32" t="str">
+        <v>6946282202</v>
       </c>
     </row>
     <row r="33">
@@ -937,14 +1147,20 @@
       <c r="B33" t="str">
         <v>ΤΣΑΡΙΔΗΣ  ΓΕΩΡΓΙΟΣ ΕΥΣΤΑΘΙΟΣ</v>
       </c>
-      <c r="E33" t="str">
+      <c r="D33" t="str">
+        <v>143110333</v>
+      </c>
+      <c r="F33" t="str">
         <v>Ν ΠΑΝΑΓΙΩΤΟΥ 29</v>
       </c>
-      <c r="F33" t="str">
+      <c r="G33" t="str">
         <v>61100</v>
       </c>
-      <c r="G33" t="str">
+      <c r="H33" t="str">
         <v>ΚΙΛΚΙΣ</v>
+      </c>
+      <c r="I33" t="str">
+        <v>2341023283</v>
       </c>
     </row>
     <row r="34">
@@ -954,14 +1170,20 @@
       <c r="B34" t="str">
         <v>ΓΟΥΛΑΣ  ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E34" t="str">
+      <c r="D34" t="str">
+        <v>119501159</v>
+      </c>
+      <c r="F34" t="str">
         <v>ΒΑΛΑΩΡΙΤΟΥ ΚΑΙ ΚΑΡΑΙΣΚΑΚΗ 12</v>
       </c>
-      <c r="F34" t="str">
+      <c r="G34" t="str">
         <v>45444</v>
       </c>
-      <c r="G34" t="str">
+      <c r="H34" t="str">
         <v>ΙΩΑΝΝΙΝΑ</v>
+      </c>
+      <c r="I34" t="str">
+        <v>2651031616</v>
       </c>
     </row>
     <row r="35">
@@ -971,14 +1193,20 @@
       <c r="B35" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΑΧΕΠΑ</v>
       </c>
-      <c r="E35" t="str">
+      <c r="D35" t="str">
+        <v>090024750</v>
+      </c>
+      <c r="F35" t="str">
         <v>ΣΤΙΛΠ ΚΥΡΙΑΚΙΔΗ 1</v>
       </c>
-      <c r="F35" t="str">
+      <c r="G35" t="str">
         <v>54636</v>
       </c>
-      <c r="G35" t="str">
+      <c r="H35" t="str">
         <v>ΘΕΣΣΑΛΟΝΙΚΗ</v>
+      </c>
+      <c r="I35" t="str">
+        <v>2313303071</v>
       </c>
     </row>
     <row r="36">
@@ -988,14 +1216,20 @@
       <c r="B36" t="str">
         <v>ΣΑΜΑΡΑ  ΚΑΛΛΙΟΠΗ</v>
       </c>
-      <c r="E36" t="str">
+      <c r="D36" t="str">
+        <v>077938473</v>
+      </c>
+      <c r="F36" t="str">
         <v>Π ΠΑΤΡΩΝ ΓΕΡΜΑΝΟΥ 3</v>
       </c>
-      <c r="F36" t="str">
+      <c r="G36" t="str">
         <v>12241</v>
       </c>
-      <c r="G36" t="str">
+      <c r="H36" t="str">
         <v>ΑΙΓΑΛΕΩ</v>
+      </c>
+      <c r="I36" t="str">
+        <v>2111824762</v>
       </c>
     </row>
     <row r="37">
@@ -1005,14 +1239,20 @@
       <c r="B37" t="str">
         <v>CC-LIT Α.Ε.</v>
       </c>
-      <c r="E37" t="str">
+      <c r="D37" t="str">
+        <v>800354523</v>
+      </c>
+      <c r="F37" t="str">
         <v>ΚΙΣΣΑΒΟΥ 2</v>
       </c>
-      <c r="F37" t="str">
+      <c r="G37" t="str">
         <v>18346</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H37" t="str">
         <v>ΜΟΣΧΑΤΟ</v>
+      </c>
+      <c r="I37" t="str">
+        <v>211 780 9180</v>
       </c>
     </row>
     <row r="38">
@@ -1022,14 +1262,20 @@
       <c r="B38" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΗΛΕΙΑΣ</v>
       </c>
-      <c r="E38" t="str">
+      <c r="D38" t="str">
+        <v>999181810</v>
+      </c>
+      <c r="F38" t="str">
         <v>ΣΥΝΤΡΙΑΔΑ ΠΥΡΓΟΥ 0</v>
       </c>
-      <c r="F38" t="str">
+      <c r="G38" t="str">
         <v>27100</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="str">
         <v>ΠΥΡΓΟΣ</v>
+      </c>
+      <c r="I38" t="str">
+        <v>2622360166</v>
       </c>
     </row>
     <row r="39">
@@ -1039,14 +1285,20 @@
       <c r="B39" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΚΟΡΙΝΘΟΥ</v>
       </c>
-      <c r="E39" t="str">
+      <c r="D39" t="str">
+        <v>999049011</v>
+      </c>
+      <c r="F39" t="str">
         <v>Λ ΑΘΗΝΩΝ 53</v>
       </c>
-      <c r="F39" t="str">
+      <c r="G39" t="str">
         <v>20100</v>
       </c>
-      <c r="G39" t="str">
+      <c r="H39" t="str">
         <v>ΚΟΡΙΝΘΟΣ</v>
+      </c>
+      <c r="I39" t="str">
+        <v>2741361816</v>
       </c>
     </row>
     <row r="40">
@@ -1056,14 +1308,23 @@
       <c r="B40" t="str">
         <v>1η ΥΠΕ - ΓΕΝ. ΟΓΚΟΛΟΓΙΚΟ ΝΟΣΟΚΟΜΕΙΟ</v>
       </c>
-      <c r="E40" t="str">
+      <c r="D40" t="str">
+        <v>998965076</v>
+      </c>
+      <c r="F40" t="str">
         <v>ΘΕΣΗ ΚΑΛΥΦΤΑΚΗ 0</v>
       </c>
-      <c r="F40" t="str">
+      <c r="G40" t="str">
         <v>14564</v>
       </c>
-      <c r="G40" t="str">
+      <c r="H40" t="str">
         <v>ΚΗΦΙΣΙΑ</v>
+      </c>
+      <c r="I40" t="str">
+        <v>2103501708</v>
+      </c>
+      <c r="J40" t="str">
+        <v>2103501809</v>
       </c>
     </row>
     <row r="41">
@@ -1073,14 +1334,20 @@
       <c r="B41" t="str">
         <v>Γ.ΝΟΣΟΚ. ΑΤΤΙΚΗΣ ΣΙΣΜΑΝΟΓΛΕΙΟ</v>
       </c>
-      <c r="E41" t="str">
+      <c r="D41" t="str">
+        <v>998986625</v>
+      </c>
+      <c r="F41" t="str">
         <v>ΤΕΡΜΑ ΣΙΣΜΑΝΟΓΛΕΙΟΥ 0</v>
       </c>
-      <c r="F41" t="str">
+      <c r="G41" t="str">
         <v>15126</v>
       </c>
-      <c r="G41" t="str">
+      <c r="H41" t="str">
         <v>ΜΑΡΟΥΣΙ</v>
+      </c>
+      <c r="I41" t="str">
+        <v>2132058405</v>
       </c>
     </row>
     <row r="42">
@@ -1090,13 +1357,16 @@
       <c r="B42" t="str">
         <v>ΕΦΚΑ - ΕΝΙΑΙΟΣ ΦΟΡΕΑΣ ΚΟΙΝΩΝΙΚΗΣ ΑΣΦΑΛΙΣ</v>
       </c>
-      <c r="E42" t="str">
+      <c r="D42" t="str">
+        <v>997072577</v>
+      </c>
+      <c r="F42" t="str">
         <v>ΑΜΕΡΙΚΗΣ 12</v>
       </c>
-      <c r="F42" t="str">
+      <c r="G42" t="str">
         <v>10671</v>
       </c>
-      <c r="G42" t="str">
+      <c r="H42" t="str">
         <v>ΑΘΗΝΑ</v>
       </c>
     </row>
@@ -1107,14 +1377,23 @@
       <c r="B43" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΠΕΛΛΑΣ</v>
       </c>
-      <c r="E43" t="str">
+      <c r="D43" t="str">
+        <v>999834338</v>
+      </c>
+      <c r="F43" t="str">
         <v>ΤΕΡΜΑ ΕΓΝΑΤΙΑΣ</v>
       </c>
-      <c r="F43" t="str">
+      <c r="G43" t="str">
         <v>58200</v>
       </c>
-      <c r="G43" t="str">
+      <c r="H43" t="str">
         <v>ΕΔΕΣΣΑ</v>
+      </c>
+      <c r="I43" t="str">
+        <v>2382350566</v>
+      </c>
+      <c r="J43" t="str">
+        <v>2382350567</v>
       </c>
     </row>
     <row r="44">
@@ -1124,14 +1403,20 @@
       <c r="B44" t="str">
         <v>ΓΕΝΙΚΟ ΝΟΣΟΚΟΜΕΙΟ ΛΑΚΩΝΙΑΣ</v>
       </c>
-      <c r="E44" t="str">
+      <c r="D44" t="str">
+        <v>999344780</v>
+      </c>
+      <c r="F44" t="str">
         <v>ΝΟΣΟΚΟΜΕΙΟ ΣΠΑΡΤΗΣ 0</v>
       </c>
-      <c r="F44" t="str">
+      <c r="G44" t="str">
         <v>23100</v>
       </c>
-      <c r="G44" t="str">
+      <c r="H44" t="str">
         <v>ΣΠΑΡΤΗ</v>
+      </c>
+      <c r="I44" t="str">
+        <v>2732360179</v>
       </c>
     </row>
     <row r="45">
@@ -1141,14 +1426,20 @@
       <c r="B45" t="str">
         <v>ΕΘΝΙΚΟΣ ΟΡΓΑΝΙΣΜΟΣ ΜΕΤΑΜΟΣΧΕΥΣΕΩΝ</v>
       </c>
-      <c r="E45" t="str">
+      <c r="D45" t="str">
+        <v>099633861</v>
+      </c>
+      <c r="F45" t="str">
         <v>ΤΣΟΧΑ 5</v>
       </c>
-      <c r="F45" t="str">
+      <c r="G45" t="str">
         <v>11521</v>
       </c>
-      <c r="G45" t="str">
+      <c r="H45" t="str">
         <v>ΑΘΗΝΑ</v>
+      </c>
+      <c r="I45" t="str">
+        <v>2132027017</v>
       </c>
     </row>
     <row r="46">
@@ -1158,14 +1449,20 @@
       <c r="B46" t="str">
         <v>Γ. ΠΑΠΑΝΙΚΟΛΑΟΥ ΝΟΣΟΚΟΜΕΙΟ ΘΕΣ/ΝΙΚΗΣ</v>
       </c>
-      <c r="E46" t="str">
+      <c r="D46" t="str">
+        <v>999294028</v>
+      </c>
+      <c r="F46" t="str">
         <v>ΕΞΟΧΗ 0</v>
       </c>
-      <c r="F46" t="str">
+      <c r="G46" t="str">
         <v>57010</v>
       </c>
-      <c r="G46" t="str">
+      <c r="H46" t="str">
         <v>ΕΞΟΧΗ</v>
+      </c>
+      <c r="I46" t="str">
+        <v>2313324112-376</v>
       </c>
     </row>
     <row r="47">
@@ -1175,14 +1472,23 @@
       <c r="B47" t="str">
         <v>ΠΑΠΑΒΑΣΙΛΕΙΟΥ  ΓΕΩΡΓΙΟΣ</v>
       </c>
-      <c r="E47" t="str">
+      <c r="D47" t="str">
+        <v>120900310</v>
+      </c>
+      <c r="F47" t="str">
         <v>ΧΙΛΗΣ 71</v>
       </c>
-      <c r="F47" t="str">
+      <c r="G47" t="str">
         <v>18755</v>
       </c>
-      <c r="G47" t="str">
+      <c r="H47" t="str">
         <v>ΚΕΡΑΤΣΙΝΙ</v>
+      </c>
+      <c r="I47" t="str">
+        <v>2130288808</v>
+      </c>
+      <c r="J47" t="str">
+        <v>6930691809</v>
       </c>
     </row>
     <row r="48">
@@ -1192,14 +1498,20 @@
       <c r="B48" t="str">
         <v>ΗΛΙΟΠΟΥΛΟΣ  ΓΕΩΡΓΙΟΣ ΕΥΣΤΑΘΙΟΣ</v>
       </c>
-      <c r="E48" t="str">
+      <c r="D48" t="str">
+        <v>106075362</v>
+      </c>
+      <c r="F48" t="str">
         <v>ΠΟΛΥΤΕΧΝΕΙΟΥ 6</v>
       </c>
-      <c r="F48" t="str">
+      <c r="G48" t="str">
         <v>50200</v>
       </c>
-      <c r="G48" t="str">
+      <c r="H48" t="str">
         <v>ΠΤΟΛΕΜΑΙΔΑ</v>
+      </c>
+      <c r="I48" t="str">
+        <v>2463080888</v>
       </c>
     </row>
     <row r="49">
@@ -1212,14 +1524,23 @@
       <c r="C49" t="str">
         <v>michael.tolis@gmail.com</v>
       </c>
-      <c r="E49" t="str">
+      <c r="D49" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="F49" t="str">
         <v>Kaiser Bridge</v>
       </c>
-      <c r="F49" t="str">
+      <c r="G49" t="str">
         <v>49100</v>
       </c>
-      <c r="G49" t="str">
+      <c r="H49" t="str">
         <v/>
+      </c>
+      <c r="I49" t="str">
+        <v>6975362321</v>
+      </c>
+      <c r="J49" t="str">
+        <v>6975362321</v>
       </c>
     </row>
     <row r="50">
@@ -1232,14 +1553,23 @@
       <c r="C50" t="str">
         <v>michael.tolis@gmail.com</v>
       </c>
-      <c r="E50" t="str">
+      <c r="D50" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="F50" t="str">
         <v>Kaiser Bridge</v>
       </c>
-      <c r="F50" t="str">
+      <c r="G50" t="str">
         <v>49100</v>
       </c>
-      <c r="G50" t="str">
+      <c r="H50" t="str">
         <v/>
+      </c>
+      <c r="I50" t="str">
+        <v>6975362321</v>
+      </c>
+      <c r="J50" t="str">
+        <v>6975362321</v>
       </c>
     </row>
     <row r="51">
@@ -1252,14 +1582,23 @@
       <c r="C51" t="str">
         <v>michael.tolis@gmail.com</v>
       </c>
-      <c r="E51" t="str">
+      <c r="D51" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="F51" t="str">
         <v>Kaiser Bridge</v>
       </c>
-      <c r="F51" t="str">
+      <c r="G51" t="str">
         <v>49100</v>
       </c>
-      <c r="G51" t="str">
+      <c r="H51" t="str">
         <v/>
+      </c>
+      <c r="I51" t="str">
+        <v>6975362321</v>
+      </c>
+      <c r="J51" t="str">
+        <v>6975362321</v>
       </c>
     </row>
     <row r="52">
@@ -1272,14 +1611,23 @@
       <c r="C52" t="str">
         <v>michael.tolis@gmail.com</v>
       </c>
-      <c r="E52" t="str">
+      <c r="D52" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="F52" t="str">
         <v>Kaiser Bridge</v>
       </c>
-      <c r="F52" t="str">
+      <c r="G52" t="str">
         <v>49100</v>
       </c>
-      <c r="G52" t="str">
+      <c r="H52" t="str">
         <v/>
+      </c>
+      <c r="I52" t="str">
+        <v>6975362321</v>
+      </c>
+      <c r="J52" t="str">
+        <v>6975362321</v>
       </c>
     </row>
     <row r="53">
@@ -1292,14 +1640,23 @@
       <c r="C53" t="str">
         <v>michael.tolis@gmail.com</v>
       </c>
-      <c r="E53" t="str">
+      <c r="D53" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="F53" t="str">
         <v>Kaiser Bridge</v>
       </c>
-      <c r="F53" t="str">
+      <c r="G53" t="str">
         <v>49100</v>
       </c>
-      <c r="G53" t="str">
+      <c r="H53" t="str">
         <v/>
+      </c>
+      <c r="I53" t="str">
+        <v>6975362321</v>
+      </c>
+      <c r="J53" t="str">
+        <v>6975362321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>